<commit_message>
book master sheet update
</commit_message>
<xml_diff>
--- a/node/simplyread-server/data/master.xlsx
+++ b/node/simplyread-server/data/master.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="20010" windowHeight="8340"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
-    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
-    <sheet name="工作表3" sheetId="3" r:id="rId3"/>
+    <sheet name="books" sheetId="1" r:id="rId1"/>
+    <sheet name="categories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>isbn</t>
   </si>
@@ -33,9 +32,6 @@
     <t>我在故宮修文物</t>
   </si>
   <si>
-    <t>社科</t>
-  </si>
-  <si>
     <t>9888365797</t>
   </si>
   <si>
@@ -108,13 +104,49 @@
     <t>9789624575316</t>
   </si>
   <si>
-    <t>宗教</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
     <t>基道書樓</t>
+  </si>
+  <si>
+    <t>商管理財</t>
+  </si>
+  <si>
+    <t>社會科學</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>20170922</t>
+  </si>
+  <si>
+    <t>流行文學</t>
+  </si>
+  <si>
+    <t>心理勵志</t>
+  </si>
+  <si>
+    <t>飲食文化</t>
+  </si>
+  <si>
+    <t>旅遊天地</t>
+  </si>
+  <si>
+    <t>生活趣味</t>
+  </si>
+  <si>
+    <t>養生保健</t>
+  </si>
+  <si>
+    <t>兒童圖書</t>
+  </si>
+  <si>
+    <t>宗教哲學</t>
+  </si>
+  <si>
+    <t>親子教育</t>
   </si>
 </sst>
 </file>
@@ -454,11 +486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -470,7 +502,7 @@
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,213 +513,318 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>categories!$A$2:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B12" sqref="B12:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="21.75" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="5" max="6" width="9" customWidth="1"/>
   </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
book data from hanlin.com
</commit_message>
<xml_diff>
--- a/node/simplyread-server/data/master.xlsx
+++ b/node/simplyread-server/data/master.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20010" windowHeight="8340"/>
+    <workbookView xWindow="6280" yWindow="1200" windowWidth="20020" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="books" sheetId="1" r:id="rId1"/>
     <sheet name="categories" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="161">
   <si>
     <t>isbn</t>
   </si>
@@ -116,9 +121,6 @@
     <t>社會科學</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>20170922</t>
   </si>
   <si>
@@ -147,16 +149,391 @@
   </si>
   <si>
     <t>親子教育</t>
+  </si>
+  <si>
+    <t>中国大历史</t>
+  </si>
+  <si>
+    <t>万历十五年</t>
+  </si>
+  <si>
+    <t>黄河青山——黄仁宇回忆录</t>
+  </si>
+  <si>
+    <t>地北天南叙古今</t>
+  </si>
+  <si>
+    <t>股票操作学（第二版）</t>
+  </si>
+  <si>
+    <t>关系千万重</t>
+  </si>
+  <si>
+    <t>进化新篇章</t>
+  </si>
+  <si>
+    <t>文化苦旅</t>
+  </si>
+  <si>
+    <t>图雅的涂鸦</t>
+  </si>
+  <si>
+    <t>赫逊河畔谈中国历史</t>
+  </si>
+  <si>
+    <t>张五常作品系列（第一辑）（共三册）</t>
+  </si>
+  <si>
+    <t>霜冷长河</t>
+  </si>
+  <si>
+    <t>我们仨</t>
+  </si>
+  <si>
+    <t>千年一叹</t>
+  </si>
+  <si>
+    <t>资本主义与二十一世纪</t>
+  </si>
+  <si>
+    <t>富萍</t>
+  </si>
+  <si>
+    <t>行者无疆</t>
+  </si>
+  <si>
+    <t>西游记（绘画本）</t>
+  </si>
+  <si>
+    <t>池莉文集7：惊世之作</t>
+  </si>
+  <si>
+    <t>沈从文经典</t>
+  </si>
+  <si>
+    <t>长恨歌</t>
+  </si>
+  <si>
+    <t>脂砚斋重评石头记甲戌校本</t>
+  </si>
+  <si>
+    <t>方舟在线</t>
+  </si>
+  <si>
+    <t>围城</t>
+  </si>
+  <si>
+    <t>张爱玲文集</t>
+  </si>
+  <si>
+    <t>水与火的缠绵</t>
+  </si>
+  <si>
+    <t>山居笔记</t>
+  </si>
+  <si>
+    <t>庄子浅说</t>
+  </si>
+  <si>
+    <t>三国演义（绘画本）</t>
+  </si>
+  <si>
+    <t>放宽历史的视界</t>
+  </si>
+  <si>
+    <t>无知者无畏</t>
+  </si>
+  <si>
+    <t>饥饿的女儿</t>
+  </si>
+  <si>
+    <t>鲁迅与我七十年</t>
+  </si>
+  <si>
+    <t>新华字典（第10版）</t>
+  </si>
+  <si>
+    <t>陈寅恪集·柳如是别传（上、中、下）</t>
+  </si>
+  <si>
+    <t>管锥编（全五册）</t>
+  </si>
+  <si>
+    <t>现代化的陷阱——当代中国的经济社会问题</t>
+  </si>
+  <si>
+    <t>音乐入门</t>
+  </si>
+  <si>
+    <t>北京城杂忆</t>
+  </si>
+  <si>
+    <t>肚大能容：中国饮食文化散记</t>
+  </si>
+  <si>
+    <t>红楼小讲</t>
+  </si>
+  <si>
+    <t>上海的风花雪月</t>
+  </si>
+  <si>
+    <t>《小说选刊》金榜小说　中篇卷（上、下）</t>
+  </si>
+  <si>
+    <t>禅宗与道家</t>
+  </si>
+  <si>
+    <t>池莉文集6：致无尽岁月</t>
+  </si>
+  <si>
+    <t>生活的艺术</t>
+  </si>
+  <si>
+    <t>尘埃落定</t>
+  </si>
+  <si>
+    <t>读词常识</t>
+  </si>
+  <si>
+    <t>洗澡</t>
+  </si>
+  <si>
+    <t>国史新论</t>
+  </si>
+  <si>
+    <t>有了快感你就喊</t>
+  </si>
+  <si>
+    <t>哈佛女孩　刘亦婷／素质培养纪实</t>
+  </si>
+  <si>
+    <t>水浒传（绘画本）</t>
+  </si>
+  <si>
+    <t>蔡志忠中国古籍经典漫画（珍藏版）</t>
+  </si>
+  <si>
+    <t>无字（全三册）</t>
+  </si>
+  <si>
+    <t>《小说月报》第七届百花奖获奖作品集</t>
+  </si>
+  <si>
+    <t>资治通鉴（全二册）</t>
+  </si>
+  <si>
+    <t>三恋</t>
+  </si>
+  <si>
+    <t>时间简史——从大爆炸到黑洞（10年修订本）</t>
+  </si>
+  <si>
+    <t>怎么爱你也不够</t>
+  </si>
+  <si>
+    <t>《小说选刊》金榜小说　短篇卷</t>
+  </si>
+  <si>
+    <t>上种红菱下种藕</t>
+  </si>
+  <si>
+    <t>三国演义（上、下）</t>
+  </si>
+  <si>
+    <t>现代汉语词典（修订本）</t>
+  </si>
+  <si>
+    <t>谈艺录（补订本）</t>
+  </si>
+  <si>
+    <t>陈寅恪集·寒柳堂集</t>
+  </si>
+  <si>
+    <t>杂忆与杂写</t>
+  </si>
+  <si>
+    <t>康熙大帝</t>
+  </si>
+  <si>
+    <t>我的精神家园——王小波杂文自选集</t>
+  </si>
+  <si>
+    <t>威尼斯日记</t>
+  </si>
+  <si>
+    <t>西方音乐的故事</t>
+  </si>
+  <si>
+    <t>说文解气</t>
+  </si>
+  <si>
+    <t>青铜时代</t>
+  </si>
+  <si>
+    <t>百年思索</t>
+  </si>
+  <si>
+    <t>溃疡：直面中国学术腐败</t>
+  </si>
+  <si>
+    <t>杨振宁文录：一位科学大师看人和这个世界</t>
+  </si>
+  <si>
+    <t>哈佛天才——用卡尔·威特法则培养出的哈佛孩子</t>
+  </si>
+  <si>
+    <t>跨过厚厚的大红门</t>
+  </si>
+  <si>
+    <t>唐浩明文集·曾国藩（共三册）</t>
+  </si>
+  <si>
+    <t>国史大纲（修订本全两册）</t>
+  </si>
+  <si>
+    <t>事林广记</t>
+  </si>
+  <si>
+    <t>周作人丰子恺儿童杂事诗图笺释</t>
+  </si>
+  <si>
+    <t>梓室余墨：陈从周随笔</t>
+  </si>
+  <si>
+    <t>历史研究（修订插图本）</t>
+  </si>
+  <si>
+    <t>我读我看</t>
+  </si>
+  <si>
+    <t>易经64卦384爻故事</t>
+  </si>
+  <si>
+    <t>今生今世——我的情感历程</t>
+  </si>
+  <si>
+    <t>GRE词汇精选</t>
+  </si>
+  <si>
+    <t>中国人史纲（上下）</t>
+  </si>
+  <si>
+    <t>胡适评传</t>
+  </si>
+  <si>
+    <t>俗世奇人</t>
+  </si>
+  <si>
+    <t>晚清的魅力</t>
+  </si>
+  <si>
+    <t>挪威的森林（全译本）</t>
+  </si>
+  <si>
+    <t>钱钟书散文</t>
+  </si>
+  <si>
+    <t>池莉文集5： 午夜起舞</t>
+  </si>
+  <si>
+    <t>口红</t>
+  </si>
+  <si>
+    <t>沈从文作品精编</t>
+  </si>
+  <si>
+    <t>宋诗选注</t>
+  </si>
+  <si>
+    <t>金庸作品集（新版·12种36册）</t>
+  </si>
+  <si>
+    <t>榆下说书</t>
+  </si>
+  <si>
+    <t>710800982X</t>
+  </si>
+  <si>
+    <t>753553354x</t>
+  </si>
+  <si>
+    <t>750631889X</t>
+  </si>
+  <si>
+    <t>750631942X</t>
+  </si>
+  <si>
+    <t>753063075X</t>
+  </si>
+  <si>
+    <t>7535710654b</t>
+  </si>
+  <si>
+    <t>710100377X</t>
+  </si>
+  <si>
+    <t>754430048X</t>
+  </si>
+  <si>
+    <t>780151419X</t>
+  </si>
+  <si>
+    <t>780676156X</t>
+  </si>
+  <si>
+    <t>720803849X</t>
+  </si>
+  <si>
+    <t>750571550X</t>
+  </si>
+  <si>
+    <t>753063139X</t>
+  </si>
+  <si>
+    <t>753390995X</t>
+  </si>
+  <si>
+    <t>20170923</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>汉林书城</t>
+  </si>
+  <si>
+    <t>7108010364</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,7 +547,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -178,15 +555,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -486,23 +915,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,10 +945,10 @@
         <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -530,10 +959,10 @@
         <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -541,13 +970,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -555,13 +984,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -569,16 +998,16 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -586,16 +1015,16 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -603,16 +1032,16 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -620,16 +1049,16 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -637,16 +1066,16 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -654,16 +1083,16 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -671,16 +1100,16 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -688,16 +1117,16 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -705,16 +1134,16 @@
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -722,17 +1151,1418 @@
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4">
+        <v>7108015412</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4">
+        <v>7108014572</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4">
+        <v>7500054459</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4">
+        <v>7108014580</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4">
+        <v>7806272011</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4">
+        <v>7800288447</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4">
+        <v>7108004496</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4">
+        <v>7801495519</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4">
+        <v>7506316501</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4">
+        <v>7108018802</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="4">
+        <v>7108009153</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="4">
+        <v>7540424222</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4">
+        <v>7801423844</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4">
+        <v>7532216462</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4">
+        <v>7539915145</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4">
+        <v>7544216381</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4">
+        <v>7506309572</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4">
+        <v>7506320207</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4">
+        <v>7810457020</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4">
+        <v>7020024750</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4">
+        <v>7539605952</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4">
+        <v>7801423968</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4">
+        <v>7805315744</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="4">
+        <v>7108012073</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4">
+        <v>7532214087</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4">
+        <v>7108014696</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="4">
+        <v>7531322013</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="4">
+        <v>7541118699</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="4">
+        <v>7544219569</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="4">
+        <v>7100039312</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="4">
+        <v>7108009455</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="4">
+        <v>7101007473</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="4">
+        <v>7507209083</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="4">
+        <v>7540426071</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="4">
+        <v>7108013525</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="4">
+        <v>7108017105</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="4">
+        <v>7200044822</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="4">
+        <v>7506314185</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4">
+        <v>7540725869</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="4">
+        <v>7309016629</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="4">
+        <v>7539912375</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="4">
+        <v>7801423089</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="4">
+        <v>7020033644</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="4">
+        <v>7101022618</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="4">
+        <v>7108002175</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="4">
+        <v>7108015358</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="4">
+        <v>7500649401</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="4">
+        <v>7532216950</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="4">
+        <v>7108013835</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="4">
+        <v>7530206370</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="4">
+        <v>7532503445</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="4">
+        <v>7533914562</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="4">
+        <v>7539913665</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="4">
+        <v>7540725850</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="4">
+        <v>7544220370</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="4">
+        <v>7020008720</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="4">
+        <v>7100017777</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="4">
+        <v>7108009382</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="4">
+        <v>7108013606</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="4">
+        <v>7535421016</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="4">
+        <v>7503915862</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="4">
+        <v>7506312905</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="4">
+        <v>7530633465</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="4">
+        <v>7532123189</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="4">
+        <v>7500646712</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="4">
+        <v>7544217973</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="4">
+        <v>7544304825</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="4">
+        <v>7020037704</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="4">
+        <v>7100017661</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="4">
+        <v>7101020097</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="4">
+        <v>7101021034</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="4">
+        <v>7108012723</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="4">
+        <v>7208033986</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="4">
+        <v>7220042892</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="4">
+        <v>7500438842</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="4">
+        <v>7501157766</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="4">
+        <v>7505707663</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="4">
+        <v>7506318776</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="4">
+        <v>7532725693</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="4">
+        <v>7539912367</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="4">
+        <v>7539914645</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="4">
+        <v>7540728310</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="4">
+        <v>7020036112</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="5">
+        <v>780655808</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="4">
+        <v>7108010313</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -743,6 +2573,9 @@
           <xm:sqref>C1:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -756,75 +2589,80 @@
       <selection activeCell="B12" sqref="B12:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="2" width="21.75" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="5" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>